<commit_message>
Added 2 customer tests
</commit_message>
<xml_diff>
--- a/buy_cd.xlsx
+++ b/buy_cd.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jasongorman\Documents\Java Projects\spec_by_example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jasongorman\WebstormProjects\spec_by_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="52">
   <si>
     <t>GIVEN</t>
   </si>
@@ -525,7 +525,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+      <selection activeCell="C9" sqref="A5:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,15 +732,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="A14:M16"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -753,12 +754,10 @@
     <col min="7" max="7" width="15.109375" customWidth="1"/>
     <col min="8" max="9" width="18.109375" customWidth="1"/>
     <col min="10" max="10" width="22.77734375" customWidth="1"/>
-    <col min="11" max="11" width="11.21875" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" customWidth="1"/>
-    <col min="13" max="13" width="45.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -766,7 +765,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -774,7 +773,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -782,7 +781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -790,50 +789,37 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="K13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -865,16 +851,10 @@
         <v>32</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M14" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -906,16 +886,10 @@
         <v>7.99</v>
       </c>
       <c r="K15">
-        <v>9</v>
-      </c>
-      <c r="L15">
         <v>6.99</v>
       </c>
-      <c r="M15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
@@ -947,13 +921,7 @@
         <v>8.99</v>
       </c>
       <c r="K16">
-        <v>4</v>
-      </c>
-      <c r="L16">
         <v>7.99</v>
-      </c>
-      <c r="M16" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>